<commit_message>
fixed loop in classifier
</commit_message>
<xml_diff>
--- a/results/wordfrequencies/Information Sciences_5_percent_most_freq_kw.xlsx
+++ b/results/wordfrequencies/Information Sciences_5_percent_most_freq_kw.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gtsueng\Anaconda3\envs\outbreak\COVID19\subtopic_classifier\results\wordfrequencies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA8E25A5-485D-43E1-8098-22F9BB96B7D5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AE7B43F-BEC2-4BD4-8017-F095272562FD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="21131" windowHeight="11368" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-93" yWindow="-93" windowWidth="21131" windowHeight="11368" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1st run, 1st pass" sheetId="1" r:id="rId1"/>
@@ -1025,9 +1025,6 @@
     <t>too generic</t>
   </si>
   <si>
-    <t>included with artificial intelligence</t>
-  </si>
-  <si>
     <t>included with bibliometrics</t>
   </si>
   <si>
@@ -1104,6 +1101,9 @@
   </si>
   <si>
     <t>epidemiological model</t>
+  </si>
+  <si>
+    <t>included with artificial intelligence, also consider removing artifical intelligence since least relevant matches do not meet criteria</t>
   </si>
 </sst>
 </file>
@@ -1946,8 +1946,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D319"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.2" x14ac:dyDescent="0.6"/>
@@ -1981,7 +1981,7 @@
         <v>39</v>
       </c>
       <c r="D2" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.6">
@@ -1995,7 +1995,7 @@
         <v>39</v>
       </c>
       <c r="D3" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.6">
@@ -2009,7 +2009,7 @@
         <v>39</v>
       </c>
       <c r="D4" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.6">
@@ -2163,7 +2163,7 @@
         <v>37</v>
       </c>
       <c r="D15" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.6">
@@ -2177,7 +2177,7 @@
         <v>37</v>
       </c>
       <c r="D16" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.6">
@@ -2191,7 +2191,7 @@
         <v>37</v>
       </c>
       <c r="D17" t="s">
-        <v>334</v>
+        <v>360</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.6">
@@ -2205,7 +2205,7 @@
         <v>37</v>
       </c>
       <c r="D18" t="s">
-        <v>334</v>
+        <v>360</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.6">
@@ -2219,7 +2219,7 @@
         <v>37</v>
       </c>
       <c r="D19" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.6">
@@ -2261,7 +2261,7 @@
         <v>37</v>
       </c>
       <c r="D22" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.6">
@@ -2317,7 +2317,7 @@
         <v>37</v>
       </c>
       <c r="D26" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.6">
@@ -2513,7 +2513,7 @@
         <v>37</v>
       </c>
       <c r="D40" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.6">
@@ -2667,7 +2667,7 @@
         <v>37</v>
       </c>
       <c r="D51" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.6">
@@ -2793,7 +2793,7 @@
         <v>37</v>
       </c>
       <c r="D60" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.6">
@@ -2807,7 +2807,7 @@
         <v>37</v>
       </c>
       <c r="D61" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.6">
@@ -2821,7 +2821,7 @@
         <v>37</v>
       </c>
       <c r="D62" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.6">
@@ -2863,7 +2863,7 @@
         <v>37</v>
       </c>
       <c r="D65" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.6">
@@ -2877,7 +2877,7 @@
         <v>37</v>
       </c>
       <c r="D66" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.6">
@@ -2989,7 +2989,7 @@
         <v>37</v>
       </c>
       <c r="D74" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.6">
@@ -3017,7 +3017,7 @@
         <v>37</v>
       </c>
       <c r="D76" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.6">
@@ -3073,7 +3073,7 @@
         <v>37</v>
       </c>
       <c r="D80" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.6">
@@ -3115,7 +3115,7 @@
         <v>37</v>
       </c>
       <c r="D83" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.6">
@@ -3129,7 +3129,7 @@
         <v>37</v>
       </c>
       <c r="D84" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.6">
@@ -3143,7 +3143,7 @@
         <v>37</v>
       </c>
       <c r="D85" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.6">
@@ -3227,7 +3227,7 @@
         <v>37</v>
       </c>
       <c r="D91" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.6">
@@ -3283,7 +3283,7 @@
         <v>37</v>
       </c>
       <c r="D95" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.6">
@@ -3297,7 +3297,7 @@
         <v>37</v>
       </c>
       <c r="D96" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.6">
@@ -3311,7 +3311,7 @@
         <v>37</v>
       </c>
       <c r="D97" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.6">
@@ -3325,7 +3325,7 @@
         <v>37</v>
       </c>
       <c r="D98" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.6">
@@ -3339,7 +3339,7 @@
         <v>37</v>
       </c>
       <c r="D99" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.6">
@@ -3353,7 +3353,7 @@
         <v>37</v>
       </c>
       <c r="D100" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.6">
@@ -3367,7 +3367,7 @@
         <v>37</v>
       </c>
       <c r="D101" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.6">
@@ -3703,7 +3703,7 @@
         <v>37</v>
       </c>
       <c r="D125" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.6">
@@ -3731,7 +3731,7 @@
         <v>37</v>
       </c>
       <c r="D127" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.6">
@@ -3745,7 +3745,7 @@
         <v>37</v>
       </c>
       <c r="D128" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.6">
@@ -3759,7 +3759,7 @@
         <v>37</v>
       </c>
       <c r="D129" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.6">
@@ -3787,7 +3787,7 @@
         <v>37</v>
       </c>
       <c r="D131" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.6">
@@ -3899,7 +3899,7 @@
         <v>37</v>
       </c>
       <c r="D139" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.6">
@@ -3913,7 +3913,7 @@
         <v>37</v>
       </c>
       <c r="D140" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.6">
@@ -4081,7 +4081,7 @@
         <v>37</v>
       </c>
       <c r="D152" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.6">
@@ -4347,7 +4347,7 @@
         <v>37</v>
       </c>
       <c r="D171" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.6">
@@ -4361,7 +4361,7 @@
         <v>37</v>
       </c>
       <c r="D172" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.6">
@@ -4529,7 +4529,7 @@
         <v>37</v>
       </c>
       <c r="D184" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.6">
@@ -4543,7 +4543,7 @@
         <v>37</v>
       </c>
       <c r="D185" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.6">
@@ -4557,7 +4557,7 @@
         <v>37</v>
       </c>
       <c r="D186" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.6">
@@ -4571,7 +4571,7 @@
         <v>37</v>
       </c>
       <c r="D187" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.6">
@@ -4627,7 +4627,7 @@
         <v>37</v>
       </c>
       <c r="D191" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.6">
@@ -4683,7 +4683,7 @@
         <v>37</v>
       </c>
       <c r="D195" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.6">
@@ -4711,7 +4711,7 @@
         <v>37</v>
       </c>
       <c r="D197" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.6">
@@ -4753,7 +4753,7 @@
         <v>37</v>
       </c>
       <c r="D200" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.6">
@@ -4767,7 +4767,7 @@
         <v>37</v>
       </c>
       <c r="D201" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.6">
@@ -4795,7 +4795,7 @@
         <v>37</v>
       </c>
       <c r="D203" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.6">
@@ -4809,7 +4809,7 @@
         <v>37</v>
       </c>
       <c r="D204" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.6">
@@ -5481,7 +5481,7 @@
         <v>37</v>
       </c>
       <c r="D252" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="253" spans="1:4" x14ac:dyDescent="0.6">
@@ -5565,7 +5565,7 @@
         <v>37</v>
       </c>
       <c r="D258" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="259" spans="1:4" x14ac:dyDescent="0.6">
@@ -6125,7 +6125,7 @@
         <v>38</v>
       </c>
       <c r="D298" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="299" spans="1:4" x14ac:dyDescent="0.6">
@@ -6371,7 +6371,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>

</xml_diff>